<commit_message>
Update with friendly agent header
</commit_message>
<xml_diff>
--- a/sec_universities.xlsx
+++ b/sec_universities.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,45 +441,40 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Campus</t>
+          <t>Endowment</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Endowment</t>
+          <t>Established</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Established</t>
+          <t>Location</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Location</t>
+          <t>Nickname</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Nickname</t>
+          <t>Sporting affiliations</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Sporting affiliations</t>
+          <t>Students</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Students</t>
+          <t>Type</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Type</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Website</t>
         </is>
@@ -493,45 +488,40 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Small city, 1,970 acres (8.0 km2)</t>
+          <t>$1.22 billion (2023)(UA only)$2.09 billion (2023)(system-wide)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>$1.22 billion (2023)(UA only)$2.09 billion (2023)(system-wide)</t>
+          <t>December 18, 1820; 204 years ago (1820-12-18)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>December 18, 1820; 204 years ago (1820-12-18)</t>
+          <t>Tuscaloosa, Alabama, United States33°12′39″N 87°32′46″W﻿ / ﻿33.21083°N 87.54611°W﻿ / 33.21083; -87.54611</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Tuscaloosa, Alabama, United States33°12′39″N 87°32′46″W﻿ / ﻿33.21083°N 87.54611°W﻿ / 33.21083; -87.54611</t>
+          <t>Crimson Tide</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Crimson Tide</t>
+          <t>NCAA Division I FBS – SEC</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>NCAA Division I FBS – SEC</t>
+          <t>42,360 (fall 2025)</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>39,622 (fall 2023)</t>
+          <t>Public research university</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
-        <is>
-          <t>Public research university</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
         <is>
           <t>www.ua.edu</t>
         </is>
@@ -545,45 +535,40 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Small city, 412 acres (1.67 km2)</t>
+          <t>$1.7 billion (FY 2021)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>$1.7 billion (FY 2021)</t>
+          <t>March 27, 1871; 154 years ago (1871-03-27)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>March 27, 1871; 153 years ago (1871-03-27)</t>
+          <t>Fayetteville, Arkansas, United States36°4′7″N 94°10′34″W﻿ / ﻿36.06861°N 94.17611°W﻿ / 36.06861; -94.17611</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Fayetteville, Arkansas, United States36°04′07″N 94°10′34″W﻿ / ﻿36.068681°N 94.176012°W﻿ / 36.068681; -94.176012</t>
+          <t>Razorbacks</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Razorbacks</t>
+          <t>NCAA Division I FBS – SEC</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>NCAA Division I FBS – SEC</t>
+          <t>34,174 (fall 2025)</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>32,140 (fall 2023)</t>
+          <t>Public land-grant research university</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
-        <is>
-          <t>Public land-grant research university</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
         <is>
           <t>uark.edu</t>
         </is>
@@ -597,45 +582,40 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Small City, 1,841 acres (7.45 km2)</t>
+          <t>$1.25 billion (FY2024)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>$1.3 billion (2024)</t>
+          <t>February 7, 1856; 169 years ago (1856-02-07)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>February 7, 1856; 169 years ago (1856-02-07)</t>
+          <t>Auburn, Alabama, United States</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Auburn, Alabama, United States</t>
+          <t>Tigers</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Tigers</t>
+          <t>NCAA Division I FBS – SEC</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>NCAA Division I FBS – SEC</t>
+          <t>34,195</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>34,195</t>
+          <t>Public land-grant research university</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
-        <is>
-          <t>Public land-grant research university</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
         <is>
           <t>auburn.edu</t>
         </is>
@@ -649,45 +629,40 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Midsize city, 2,000 acres (810 ha)</t>
+          <t>$2.337 billion (2023)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>$2.337 billion (2023)</t>
+          <t>January 6, 1853;172 years ago (1853-01-06)[note 2]</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>January 6, 1853;172 years ago (1853-01-06)[note 2]</t>
+          <t>Gainesville, Florida, United States29°38′51″N 82°20′42″W﻿ / ﻿29.6475°N 82.3450°W﻿ / 29.6475; -82.3450</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Gainesville, Florida, United States29°38′51″N 82°20′42″W﻿ / ﻿29.6475°N 82.3450°W﻿ / 29.6475; -82.3450</t>
+          <t>Gators</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Gators</t>
+          <t>NCAA Division I FBS – SECBig 12</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>NCAA Division I FBS – SECBig 12</t>
+          <t>54,814 (fall 2023)</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>54,814 (fall 2023)</t>
+          <t>Public land-grant research university</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
-        <is>
-          <t>Public land-grant research university</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
         <is>
           <t>ufl.edu</t>
         </is>
@@ -701,45 +676,40 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Midsize city / College town, 762 acres (3.08 km2) (main campus)41,539 acres (168.10 km2) (total)</t>
+          <t>$2.056 billion (2024)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>$1.82 billion (2023)</t>
+          <t>January 27, 1785; 240 years ago (1785-01-27)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>January 27, 1785; 240 years ago (1785-01-27)</t>
+          <t>Athens, Georgia, US33°57′21″N 83°22′28″W﻿ / ﻿33.9558°N 83.3745°W﻿ / 33.9558; -83.3745</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Athens, Georgia, United States33°57′21″N 83°22′28″W﻿ / ﻿33.9558°N 83.3745°W﻿ / 33.9558; -83.3745</t>
+          <t>Bulldogs</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Bulldogs</t>
+          <t>NCAA Division I FBS – SEC</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>NCAA Division I FBS – SEC</t>
+          <t>40,607 (fall 2022)</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>40,607 (fall 2022)</t>
+          <t>Public flagship land-grant research university</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
-        <is>
-          <t>Public flagship land-grant research university</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
         <is>
           <t>uga.edu</t>
         </is>
@@ -753,45 +723,40 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Large City, 784 acres (3.17 km2)</t>
+          <t>$2.27 billion (2024)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>$2.13 billion (2023)</t>
+          <t>February 22, 1865;160 years ago (1865-02-22)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>February 22, 1865; 160 years ago (February 22, 1865)</t>
+          <t>Lexington, Kentucky, United States38°01′57″N 84°30′09″W﻿ / ﻿38.03250°N 84.50250°W﻿ / 38.03250; -84.50250</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Lexington, Kentucky, United States38°01′57″N 84°30′09″W﻿ / ﻿38.03250°N 84.50250°W﻿ / 38.03250; -84.50250</t>
+          <t>Wildcats</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Wildcats</t>
+          <t>NCAA Division I FBS – SECC-USAGARC</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>NCAA Division I FBS – SECC-USAGARC</t>
+          <t>35,952 (fall 2024)</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>35,952 (fall 2024)</t>
+          <t>Public land-grant research university</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
-        <is>
-          <t>Public land-grant research university</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
         <is>
           <t>uky.edu</t>
         </is>
@@ -805,45 +770,40 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Midsize city, 4,925 acres (1,993 ha)</t>
+          <t>$664.20 million (2023)(LSU only)$1.06 billion (2023)(system-wide)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>$664.20 million (2023)(LSU only)$1.06 billion (2023)(system-wide)</t>
+          <t>January 2, 1860; 165 years ago (January 2, 1860)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>January 2, 1860; 165 years ago (January 2, 1860)</t>
+          <t>Baton Rouge, Louisiana, United States30°24′52″N 91°10′42″W﻿ / ﻿30.4145°N 91.17826°W﻿ / 30.4145; -91.17826</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Baton Rouge, Louisiana, United States30°24′52″N 91°10′42″W﻿ / ﻿30.4145°N 91.17826°W﻿ / 30.4145; -91.17826</t>
+          <t>Tigers and Lady Tigers</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Tigers and Lady Tigers</t>
+          <t>NCAA Division I FBS – SECCCSA</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>NCAA Division I FBS – SECCCSA</t>
+          <t>42,016 (fall 2024)</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>37,354 (fall 2022)</t>
+          <t>Public land-grant research university</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
-        <is>
-          <t>Public land-grant research university</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
         <is>
           <t>lsu.edu</t>
         </is>
@@ -857,45 +817,40 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Remote town, 3,497 acres (14.15 km2)</t>
+          <t>$1 billion (2025)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>$962 million (2024)</t>
+          <t>February 24, 1844; 181 years ago (February 24, 1844)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>February 24, 1844; 181 years ago (February 24, 1844)</t>
+          <t>Oxford, Mississippi</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>University, Mississippi, 38677</t>
+          <t>Rebels</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Rebels</t>
+          <t>NCAA Division I FBS – SECPRC</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>NCAA Division I FBS – SECPRC</t>
+          <t>27,124</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>24,710 (for 2023-2024 year)</t>
+          <t>Public research university</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
-        <is>
-          <t>Public research university</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
         <is>
           <t>olemiss.edu</t>
         </is>
@@ -909,45 +864,40 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Remote town, 4,200 acres (17 km2)</t>
+          <t>$1.0 billion (2024)</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>$894.5 million (2024)</t>
+          <t>February 28, 1878; 147 years ago (February 28, 1878)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>February 28, 1878; 147 years ago (February 28, 1878)</t>
+          <t>Mississippi State, Mississippi, United States33°27′14″N 88°47′20″W﻿ / ﻿33.454°N 88.789°W﻿ / 33.454; -88.789</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Mississippi State, Mississippi, United States33°27′14″N 88°47′20″W﻿ / ﻿33.454°N 88.789°W﻿ / 33.454; -88.789</t>
+          <t>Bulldogs</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Bulldogs</t>
+          <t>NCAA Division I FBS – SEC</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>NCAA Division I FBS – SEC</t>
+          <t>23,150 (fall 2024)</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>23,150 (fall 2024)</t>
+          <t>Public land-grant research university</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
-        <is>
-          <t>Public land-grant research university</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
         <is>
           <t>msstate.edu</t>
         </is>
@@ -961,45 +911,40 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Midsize city, 1,262 acres (511 ha)Total, 19,261 acres (7,795 ha)</t>
+          <t>$1.42 billion (2023)(MU only)$2.24 billion (2023)(system-wide)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>$1.42 billion (2023)(MU only)$2.24 billion (2023)(system-wide)</t>
+          <t>February 11, 1839; 186 years ago (1839-02-11)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>February 11, 1839; 186 years ago (1839-02-11)</t>
+          <t>Columbia, Missouri, United States38°56′43″N 92°19′44″W﻿ / ﻿38.9453°N 92.3288°W﻿ / 38.9453; -92.3288</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Columbia, Missouri, United States38°56′43″N 92°19′44″W﻿ / ﻿38.9453°N 92.3288°W﻿ / 38.9453; -92.3288</t>
+          <t>Tigers</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Tigers</t>
+          <t>NCAA Division I FBS – SECBig 12</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>NCAA Division I FBS – SECBig 12</t>
+          <t>31,543 (fall 2024)</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>31,543 (fall 2024)</t>
+          <t>Public land-grant research university</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
-        <is>
-          <t>Public land-grant research university</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
         <is>
           <t>missouri.edu</t>
         </is>
@@ -1013,45 +958,40 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Midsize suburb, 3,000 acres (12.1 km2)</t>
+          <t>$1.81 billion (FY2024)</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>$1.81 billion (FY2024)</t>
+          <t>December 19, 1890; 134 years ago (December 19, 1890)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>December 19, 1890; 134 years ago (December 19, 1890)</t>
+          <t>Norman, Oklahoma, United States35°12′32″N 97°26′45″W﻿ / ﻿35.2088°N 97.4457°W﻿ / 35.2088; -97.4457</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Norman, Oklahoma, United States35°12′32″N 97°26′45″W﻿ / ﻿35.2088°N 97.4457°W﻿ / 35.2088; -97.4457</t>
+          <t>Sooners</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Sooners</t>
+          <t>NCAA Division I FBS – SECBig 12MPSF</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>NCAA Division I FBS - SECBig 12MPSF</t>
+          <t>34,523 (fall 2024)Norman: 30,873HSC: 3,684Tulsa: 1,127</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>34,523 (fall 2024)Norman: 30,873HSC: 3,684Tulsa: 1,127</t>
+          <t>Public research university</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
-        <is>
-          <t>Public research university</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
         <is>
           <t>ou.edu</t>
         </is>
@@ -1065,45 +1005,40 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Midsize city, 359 acres (145 ha)</t>
+          <t>$1.044 billion (2024)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>$1.044 billion (2024)</t>
+          <t>December 19, 1801; 223 years ago (1801-12-19)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>December 19, 1801; 223 years ago (1801-12-19)</t>
+          <t>Columbia, South Carolina, United States</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Columbia, South Carolina, United States</t>
+          <t>Gamecocks</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Gamecocks</t>
+          <t>NCAA Division I FBS – SEC</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>NCAA Division I FBS – SEC</t>
+          <t>&gt;38,000 (2024) (Columbia)52,633 (system-wide)</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>&gt;38,000 (2024) (Columbia)52,633 (system-wide)</t>
+          <t>Public research university</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
-        <is>
-          <t>Public research university</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
         <is>
           <t>sc.edu</t>
         </is>
@@ -1117,45 +1052,40 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Midsize city, 600 acres (240 ha)Total, 2,128 acres (861 ha)</t>
+          <t>$1.01 billion (2023)(UT Knoxville only)$1.60 billion (2023)(system-wide)</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>$1.01 billion (2023)(UT Knoxville only)$1.60 billion (2023)(system-wide)</t>
+          <t>September 10, 1794; 231 years ago (1794-09-10)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>September 10, 1794; 230 years ago (1794-09-10)</t>
+          <t>Knoxville, Tennessee, United States35°57′6″N 83°55′48″W﻿ / ﻿35.95167°N 83.93000°W﻿ / 35.95167; -83.93000</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Knoxville, Tennessee, United States35°57′6″N 83°55′48″W﻿ / ﻿35.95167°N 83.93000°W﻿ / 35.95167; -83.93000</t>
+          <t>Volunteers &amp; Lady Volunteers</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Volunteers &amp; Lady Volunteers</t>
+          <t>NCAA Division I FBS – SEC</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>NCAA Division I FBS – SEC</t>
+          <t>40,784 (fall 2025)</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>38,728 (fall 2024)</t>
+          <t>Public land-grant research university</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
-        <is>
-          <t>Public land-grant research university</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
         <is>
           <t>utk.edu</t>
         </is>
@@ -1169,45 +1099,40 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Large city, 431 acres (1.74 km2)</t>
+          <t>$20.85 billion (FY2024)(UT Austin only)$47.47 billion (FY2024)(system-wide)</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>$19.72 billion (FY2023)(UT Austin only)$47.47 billion (FY2024)(system-wide)</t>
+          <t>September 15, 1883; 142 years ago (1883-09-15)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>September 15, 1883; 141 years ago (1883-09-15)</t>
+          <t>Austin, Texas, United States30°17′06″N 97°44′06″W﻿ / ﻿30.285°N 97.735°W﻿ / 30.285; -97.735</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Austin, Texas, United States30°17′06″N 97°44′06″W﻿ / ﻿30.285°N 97.735°W﻿ / 30.285; -97.735</t>
+          <t>Longhorns</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Longhorns</t>
+          <t>NCAA Division I FBS - SEC</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>NCAA Division I FBS - SEC</t>
+          <t>53,864 (fall 2024)</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>53,082 (fall 2023)</t>
+          <t>Public research university</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
-        <is>
-          <t>Public research university</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
         <is>
           <t>utexas.edu</t>
         </is>
@@ -1221,45 +1146,40 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Midsize city, 5,500 acres (20 km2)</t>
+          <t>$18.13 billion (FY2023)(Texas A&amp;M only)$20.38 billion (FY2024)(system-wide)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>$18.13 billion (FY2023)(Texas A&amp;M only)$20.38 billion (FY2024)(system-wide)</t>
+          <t>1876; 149 years ago (1876)[note 2]</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1876; 149 years ago (1876)[note 2]</t>
+          <t>College Station, Texas, United States[note 3]30°36′37″N 96°20′37″W﻿ / ﻿30.61028°N 96.34361°W﻿ / 30.61028; -96.34361</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>College Station, Texas, United States[note 3]30°36′37″N 96°20′37″W﻿ / ﻿30.61028°N 96.34361°W﻿ / 30.61028; -96.34361</t>
+          <t>Aggies, Texas Aggies</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Aggies, Texas Aggies</t>
+          <t>NCAA Division I FBS – SEC</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>NCAA Division I FBS – SEC</t>
+          <t>79,114 (fall 2024) • 71,045 (College Station) • 2,138 (Galveston) • 1,751 (Fort Worth) • 430 (McAllen) • 3,750 (Health Science Center)</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>79,114 (fall 2024)</t>
+          <t>Public land-grant research senior military university</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
-        <is>
-          <t>Public land-grant research senior military university</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
         <is>
           <t>tamu.edu</t>
         </is>
@@ -1273,45 +1193,40 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Large city, 330 acres (1.3 km2)</t>
+          <t>$10.2 billion (2024)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>$9.7 billion (2023)</t>
+          <t>1873; 152 years ago (1873)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1873; 152 years ago (1873)</t>
+          <t>Nashville, Tennessee, United States36°8′51″N 86°48′9″W﻿ / ﻿36.14750°N 86.80250°W﻿ / 36.14750; -86.80250</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Nashville, Tennessee, United States36°8′51″N 86°48′9″W﻿ / ﻿36.14750°N 86.80250°W﻿ / 36.14750; -86.80250</t>
+          <t>Commodores</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Commodores</t>
+          <t>NCAA Division I FBS – SECThe AmericanCUSA</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>NCAA Division I FBS – SECThe AmericanCUSA</t>
+          <t>13,575 (2024)</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>13,575 (2024)</t>
+          <t>Private research university</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
-        <is>
-          <t>Private research university</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
         <is>
           <t>vanderbilt.edu</t>
         </is>

</xml_diff>